<commit_message>
Reduction silicate on Dardanelles -- used in Reanalysis 24
</commit_message>
<xml_diff>
--- a/Perseus-4.6_40rivers_genericmesh.xlsx
+++ b/Perseus-4.6_40rivers_genericmesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7840" yWindow="1020" windowWidth="31380" windowHeight="22580" tabRatio="992" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" tabRatio="992" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="monthly" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,14 @@
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -79,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="80">
   <si>
     <t>ID</t>
   </si>
@@ -315,14 +323,41 @@
   <si>
     <t>mmol/m3</t>
   </si>
+  <si>
+    <t>LEV</t>
+  </si>
+  <si>
+    <t>NWM</t>
+  </si>
+  <si>
+    <t>ADR</t>
+  </si>
+  <si>
+    <t>DARD</t>
+  </si>
+  <si>
+    <t>TYR</t>
+  </si>
+  <si>
+    <t>AEG</t>
+  </si>
+  <si>
+    <t>ION</t>
+  </si>
+  <si>
+    <t>SWM</t>
+  </si>
+  <si>
+    <t>EAST</t>
+  </si>
+  <si>
+    <t>WEST</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000"/>
-  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -355,12 +390,24 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -393,7 +440,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -402,7 +449,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -499,16 +547,19 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rivers_lon_lat" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rivers_lon_lat_1" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rivers_lon_lat_1" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rivers_lon_lat" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -836,7 +887,7 @@
   <dimension ref="A1:X57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F2" sqref="F2:F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4848,13 +4899,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB57"/>
+  <dimension ref="A1:BB64"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView topLeftCell="A21" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60:BB64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="15.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -5030,6 +5084,15 @@
       <c r="E2">
         <v>33</v>
       </c>
+      <c r="F2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J2">
         <v>1.7396</v>
       </c>
@@ -5179,6 +5242,15 @@
       <c r="E3">
         <v>34</v>
       </c>
+      <c r="F3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J3">
         <v>1.7396</v>
       </c>
@@ -5328,6 +5400,15 @@
       <c r="E4">
         <v>254</v>
       </c>
+      <c r="F4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="J4">
         <v>1.0105</v>
       </c>
@@ -5477,6 +5558,15 @@
       <c r="E5">
         <v>358</v>
       </c>
+      <c r="F5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J5">
         <v>0.25871</v>
       </c>
@@ -5626,6 +5716,15 @@
       <c r="E6">
         <v>357</v>
       </c>
+      <c r="F6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J6">
         <v>0.61516000000000004</v>
       </c>
@@ -5775,6 +5874,15 @@
       <c r="E7">
         <v>356</v>
       </c>
+      <c r="F7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J7">
         <v>1.7304999999999999</v>
       </c>
@@ -5924,6 +6032,15 @@
       <c r="E8">
         <v>355</v>
       </c>
+      <c r="F8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J8">
         <v>0.53466999999999998</v>
       </c>
@@ -6073,6 +6190,15 @@
       <c r="E9">
         <v>354</v>
       </c>
+      <c r="F9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J9">
         <v>0.24146999999999999</v>
       </c>
@@ -6222,6 +6348,15 @@
       <c r="E10">
         <v>353</v>
       </c>
+      <c r="F10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J10">
         <v>0.87963000000000002</v>
       </c>
@@ -6371,6 +6506,15 @@
       <c r="E11">
         <v>351</v>
       </c>
+      <c r="F11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" t="s">
+        <v>72</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J11">
         <v>0.91412000000000004</v>
       </c>
@@ -6520,6 +6664,15 @@
       <c r="E12">
         <v>351</v>
       </c>
+      <c r="F12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" t="s">
+        <v>72</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J12">
         <v>0.57491999999999999</v>
       </c>
@@ -6669,6 +6822,15 @@
       <c r="E13">
         <v>359</v>
       </c>
+      <c r="F13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J13">
         <v>8.3542000000000005E-2</v>
       </c>
@@ -6818,6 +6980,15 @@
       <c r="E14">
         <v>351</v>
       </c>
+      <c r="F14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" t="s">
+        <v>72</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J14">
         <v>2.3167E-2</v>
       </c>
@@ -6967,6 +7138,15 @@
       <c r="E15">
         <v>316</v>
       </c>
+      <c r="F15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="J15">
         <v>5.3255999999999997</v>
       </c>
@@ -7116,6 +7296,15 @@
       <c r="E16">
         <v>319</v>
       </c>
+      <c r="F16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" t="s">
+        <v>71</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="J16">
         <v>0.59174000000000004</v>
       </c>
@@ -7265,6 +7454,15 @@
       <c r="E17">
         <v>252</v>
       </c>
+      <c r="F17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" t="s">
+        <v>72</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J17">
         <v>0.28267999999999999</v>
       </c>
@@ -7414,6 +7612,15 @@
       <c r="E18">
         <v>256</v>
       </c>
+      <c r="F18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" t="s">
+        <v>72</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J18">
         <v>0.29533999999999999</v>
       </c>
@@ -7563,6 +7770,15 @@
       <c r="E19">
         <v>280</v>
       </c>
+      <c r="F19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" t="s">
+        <v>72</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J19">
         <v>0.59763999999999995</v>
       </c>
@@ -7712,6 +7928,15 @@
       <c r="E20">
         <v>281</v>
       </c>
+      <c r="F20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20" t="s">
+        <v>72</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J20">
         <v>0.59763999999999995</v>
       </c>
@@ -7861,6 +8086,12 @@
       <c r="E21">
         <v>238</v>
       </c>
+      <c r="F21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21" t="s">
+        <v>73</v>
+      </c>
       <c r="J21">
         <v>0.2</v>
       </c>
@@ -8010,6 +8241,12 @@
       <c r="E22">
         <v>237</v>
       </c>
+      <c r="F22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22" t="s">
+        <v>73</v>
+      </c>
       <c r="J22">
         <v>0.2</v>
       </c>
@@ -8159,6 +8396,12 @@
       <c r="E23">
         <v>236</v>
       </c>
+      <c r="F23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23" t="s">
+        <v>73</v>
+      </c>
       <c r="J23">
         <v>0.2</v>
       </c>
@@ -8308,6 +8551,15 @@
       <c r="E24">
         <v>369</v>
       </c>
+      <c r="F24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G24" t="s">
+        <v>72</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J24">
         <v>0.13306999999999999</v>
       </c>
@@ -8457,6 +8709,15 @@
       <c r="E25">
         <v>372</v>
       </c>
+      <c r="F25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G25" t="s">
+        <v>72</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J25">
         <v>0.16617999999999999</v>
       </c>
@@ -8606,6 +8867,15 @@
       <c r="E26">
         <v>374</v>
       </c>
+      <c r="F26" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G26" t="s">
+        <v>72</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J26">
         <v>9.3745999999999996E-2</v>
       </c>
@@ -8755,6 +9025,15 @@
       <c r="E27">
         <v>370</v>
       </c>
+      <c r="F27" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J27">
         <v>0.31674999999999998</v>
       </c>
@@ -8904,6 +9183,15 @@
       <c r="E28">
         <v>361</v>
       </c>
+      <c r="F28" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G28" t="s">
+        <v>72</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J28">
         <v>1.5596000000000001</v>
       </c>
@@ -9053,6 +9341,15 @@
       <c r="E29">
         <v>360</v>
       </c>
+      <c r="F29" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G29" t="s">
+        <v>72</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J29">
         <v>0.46617999999999998</v>
       </c>
@@ -9202,6 +9499,15 @@
       <c r="E30">
         <v>347</v>
       </c>
+      <c r="F30" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G30" t="s">
+        <v>72</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J30">
         <v>4.1383999999999997E-2</v>
       </c>
@@ -9351,6 +9657,15 @@
       <c r="E31">
         <v>347</v>
       </c>
+      <c r="F31" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G31" t="s">
+        <v>72</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J31">
         <v>0.58245000000000002</v>
       </c>
@@ -9500,6 +9815,15 @@
       <c r="E32">
         <v>324</v>
       </c>
+      <c r="F32" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G32" t="s">
+        <v>72</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J32">
         <v>5.9698000000000001E-2</v>
       </c>
@@ -9649,6 +9973,15 @@
       <c r="E33">
         <v>325</v>
       </c>
+      <c r="F33" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G33" t="s">
+        <v>74</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="J33">
         <v>6.2678000000000003</v>
       </c>
@@ -9798,6 +10131,15 @@
       <c r="E34">
         <v>309</v>
       </c>
+      <c r="F34" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G34" t="s">
+        <v>72</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J34">
         <v>6.6848000000000005E-2</v>
       </c>
@@ -9947,6 +10289,15 @@
       <c r="E35">
         <v>313</v>
       </c>
+      <c r="F35" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G35" t="s">
+        <v>71</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="J35">
         <v>0.26852999999999999</v>
       </c>
@@ -10096,6 +10447,15 @@
       <c r="E36">
         <v>298</v>
       </c>
+      <c r="F36" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G36" t="s">
+        <v>75</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J36">
         <v>1.4645E-2</v>
       </c>
@@ -10245,6 +10605,15 @@
       <c r="E37">
         <v>278</v>
       </c>
+      <c r="F37" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G37" t="s">
+        <v>74</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="J37">
         <v>0.67776999999999998</v>
       </c>
@@ -10394,6 +10763,15 @@
       <c r="E38">
         <v>279</v>
       </c>
+      <c r="F38" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G38" t="s">
+        <v>74</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="J38">
         <v>0.67776999999999998</v>
       </c>
@@ -10543,6 +10921,15 @@
       <c r="E39">
         <v>276</v>
       </c>
+      <c r="F39" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G39" t="s">
+        <v>75</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J39">
         <v>8.9215000000000003E-2</v>
       </c>
@@ -10692,6 +11079,15 @@
       <c r="E40">
         <v>261</v>
       </c>
+      <c r="F40" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G40" t="s">
+        <v>74</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="J40">
         <v>0.51256999999999997</v>
       </c>
@@ -10841,6 +11237,15 @@
       <c r="E41">
         <v>261</v>
       </c>
+      <c r="F41" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G41" t="s">
+        <v>75</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J41">
         <v>7.2150000000000006E-2</v>
       </c>
@@ -10990,6 +11395,15 @@
       <c r="E42">
         <v>255</v>
       </c>
+      <c r="F42" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G42" t="s">
+        <v>75</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J42">
         <v>1.7317</v>
       </c>
@@ -11139,6 +11553,15 @@
       <c r="E43">
         <v>254</v>
       </c>
+      <c r="F43" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G43" t="s">
+        <v>75</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J43">
         <v>2.4813999999999998</v>
       </c>
@@ -11288,6 +11711,15 @@
       <c r="E44">
         <v>248</v>
       </c>
+      <c r="F44" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G44" t="s">
+        <v>75</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J44">
         <v>2.0872000000000002</v>
       </c>
@@ -11437,6 +11869,15 @@
       <c r="E45">
         <v>213</v>
       </c>
+      <c r="F45" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G45" t="s">
+        <v>76</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J45">
         <v>5.3858999999999997E-2</v>
       </c>
@@ -11586,6 +12027,15 @@
       <c r="E46">
         <v>235</v>
       </c>
+      <c r="F46" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G46" t="s">
+        <v>75</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J46">
         <v>0.71128999999999998</v>
       </c>
@@ -11735,6 +12185,15 @@
       <c r="E47">
         <v>197</v>
       </c>
+      <c r="F47" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G47" t="s">
+        <v>76</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J47">
         <v>9.9788000000000002E-2</v>
       </c>
@@ -11884,6 +12343,15 @@
       <c r="E48">
         <v>203</v>
       </c>
+      <c r="F48" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G48" t="s">
+        <v>75</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J48">
         <v>0.28671999999999997</v>
       </c>
@@ -12033,6 +12501,15 @@
       <c r="E49">
         <v>177</v>
       </c>
+      <c r="F49" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G49" t="s">
+        <v>75</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J49">
         <v>0.14665</v>
       </c>
@@ -12182,6 +12659,15 @@
       <c r="E50">
         <v>160</v>
       </c>
+      <c r="F50" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G50" t="s">
+        <v>70</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J50">
         <v>0.11157</v>
       </c>
@@ -12331,6 +12817,15 @@
       <c r="E51">
         <v>158</v>
       </c>
+      <c r="F51" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G51" t="s">
+        <v>70</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J51">
         <v>0.15803</v>
       </c>
@@ -12480,6 +12975,15 @@
       <c r="E52">
         <v>158</v>
       </c>
+      <c r="F52" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G52" t="s">
+        <v>70</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J52">
         <v>1.6794</v>
       </c>
@@ -12629,6 +13133,15 @@
       <c r="E53">
         <v>154</v>
       </c>
+      <c r="F53" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G53" t="s">
+        <v>70</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J53">
         <v>0.49091000000000001</v>
       </c>
@@ -12778,6 +13291,15 @@
       <c r="E54">
         <v>147</v>
       </c>
+      <c r="F54" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G54" t="s">
+        <v>70</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J54">
         <v>0.26174999999999998</v>
       </c>
@@ -12927,6 +13449,15 @@
       <c r="E55">
         <v>165</v>
       </c>
+      <c r="F55" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G55" t="s">
+        <v>77</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="J55">
         <v>0.14374999999999999</v>
       </c>
@@ -13076,6 +13607,15 @@
       <c r="E56">
         <v>142</v>
       </c>
+      <c r="F56" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G56" t="s">
+        <v>70</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J56">
         <v>0.18185999999999999</v>
       </c>
@@ -13380,6 +13920,561 @@
       <c r="BB57">
         <f>KM3perYR_NOBLS!AZ57</f>
         <v>-999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="I60" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="J60">
+        <f>SUM(J2:J3,J5:J14,J17:J20,J24:J32,J34,J36,J39,J41:J54,J56)</f>
+        <v>25.252432000000002</v>
+      </c>
+      <c r="K60">
+        <f t="shared" ref="K60:AX60" si="4">SUM(K2:K3,K5:K14,K17:K20,K24:K32,K34,K36,K39,K41:K54,K56)</f>
+        <v>22.848344999999998</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="4"/>
+        <v>23.931396000000007</v>
+      </c>
+      <c r="M60">
+        <f t="shared" si="4"/>
+        <v>24.233692999999992</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="4"/>
+        <v>26.89252999999999</v>
+      </c>
+      <c r="O60">
+        <f t="shared" si="4"/>
+        <v>21.384519500000003</v>
+      </c>
+      <c r="P60">
+        <f t="shared" si="4"/>
+        <v>22.888135599999995</v>
+      </c>
+      <c r="Q60">
+        <f t="shared" si="4"/>
+        <v>21.446458699999997</v>
+      </c>
+      <c r="R60">
+        <f t="shared" si="4"/>
+        <v>20.713224699999998</v>
+      </c>
+      <c r="S60">
+        <f t="shared" si="4"/>
+        <v>19.688266499999997</v>
+      </c>
+      <c r="T60">
+        <f t="shared" si="4"/>
+        <v>15.208548800000001</v>
+      </c>
+      <c r="U60">
+        <f t="shared" si="4"/>
+        <v>23.811131000000003</v>
+      </c>
+      <c r="V60">
+        <f t="shared" si="4"/>
+        <v>19.141209199999995</v>
+      </c>
+      <c r="W60">
+        <f t="shared" si="4"/>
+        <v>19.196113399999998</v>
+      </c>
+      <c r="X60">
+        <f t="shared" si="4"/>
+        <v>21.070329999999995</v>
+      </c>
+      <c r="Y60">
+        <f t="shared" si="4"/>
+        <v>19.835535999999994</v>
+      </c>
+      <c r="Z60">
+        <f t="shared" si="4"/>
+        <v>19.488231000000003</v>
+      </c>
+      <c r="AA60">
+        <f t="shared" si="4"/>
+        <v>17.956840700000004</v>
+      </c>
+      <c r="AB60">
+        <f t="shared" si="4"/>
+        <v>21.268274600000005</v>
+      </c>
+      <c r="AC60">
+        <f t="shared" si="4"/>
+        <v>20.812713600000002</v>
+      </c>
+      <c r="AD60">
+        <f t="shared" si="4"/>
+        <v>20.513940700000003</v>
+      </c>
+      <c r="AE60">
+        <f t="shared" si="4"/>
+        <v>17.128386299999999</v>
+      </c>
+      <c r="AF60">
+        <f t="shared" si="4"/>
+        <v>19.950705700000007</v>
+      </c>
+      <c r="AG60">
+        <f t="shared" si="4"/>
+        <v>21.754835100000008</v>
+      </c>
+      <c r="AH60">
+        <f t="shared" si="4"/>
+        <v>21.635482700000001</v>
+      </c>
+      <c r="AI60">
+        <f t="shared" si="4"/>
+        <v>21.736114200000003</v>
+      </c>
+      <c r="AJ60">
+        <f t="shared" si="4"/>
+        <v>18.627535300000002</v>
+      </c>
+      <c r="AK60">
+        <f t="shared" si="4"/>
+        <v>24.798399499999999</v>
+      </c>
+      <c r="AL60">
+        <f t="shared" si="4"/>
+        <v>25.564343699999991</v>
+      </c>
+      <c r="AM60">
+        <f t="shared" si="4"/>
+        <v>20.788269499999995</v>
+      </c>
+      <c r="AN60">
+        <f t="shared" si="4"/>
+        <v>20.246228500000004</v>
+      </c>
+      <c r="AO60">
+        <f t="shared" si="4"/>
+        <v>17.592565999999994</v>
+      </c>
+      <c r="AP60">
+        <f t="shared" si="4"/>
+        <v>20.018779599999998</v>
+      </c>
+      <c r="AQ60">
+        <f t="shared" si="4"/>
+        <v>22.289102699999994</v>
+      </c>
+      <c r="AR60">
+        <f t="shared" si="4"/>
+        <v>19.537418500000001</v>
+      </c>
+      <c r="AS60">
+        <f t="shared" si="4"/>
+        <v>18.209973299999998</v>
+      </c>
+      <c r="AT60">
+        <f t="shared" si="4"/>
+        <v>21.207163899999998</v>
+      </c>
+      <c r="AU60">
+        <f t="shared" si="4"/>
+        <v>24.9599309</v>
+      </c>
+      <c r="AV60">
+        <f t="shared" si="4"/>
+        <v>24.111951999999999</v>
+      </c>
+      <c r="AW60">
+        <f t="shared" si="4"/>
+        <v>26.487925999999995</v>
+      </c>
+      <c r="AX60">
+        <f t="shared" si="4"/>
+        <v>23.253758300000005</v>
+      </c>
+      <c r="AZ60">
+        <f t="shared" ref="AZ60:BB60" si="5">SUM(AZ2:AZ3,AZ5:AZ14,AZ17:AZ20,AZ24:AZ32,AZ34,AZ36,AZ39,AZ41:AZ54,AZ56)</f>
+        <v>21.15856738181818</v>
+      </c>
+      <c r="BA60">
+        <f t="shared" si="5"/>
+        <v>133.76680795816952</v>
+      </c>
+      <c r="BB60">
+        <f t="shared" si="5"/>
+        <v>198.85098909090908</v>
+      </c>
+    </row>
+    <row r="61" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="I61" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="J61">
+        <f>SUM(J4,J15:J16,J33,J35,J37:J38,J40,J55)</f>
+        <v>15.476030000000003</v>
+      </c>
+      <c r="K61">
+        <f t="shared" ref="K61:AX61" si="6">SUM(K4,K15:K16,K33,K35,K37:K38,K40,K55)</f>
+        <v>13.439310000000003</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="6"/>
+        <v>17.874889000000003</v>
+      </c>
+      <c r="M61">
+        <f t="shared" si="6"/>
+        <v>17.581619999999997</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="6"/>
+        <v>18.460190000000001</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="6"/>
+        <v>18.583159999999996</v>
+      </c>
+      <c r="P61">
+        <f t="shared" si="6"/>
+        <v>20.522190000000002</v>
+      </c>
+      <c r="Q61">
+        <f t="shared" si="6"/>
+        <v>15.21557</v>
+      </c>
+      <c r="R61">
+        <f t="shared" si="6"/>
+        <v>13.970400000000001</v>
+      </c>
+      <c r="S61">
+        <f t="shared" si="6"/>
+        <v>9.6076600000000028</v>
+      </c>
+      <c r="T61">
+        <f t="shared" si="6"/>
+        <v>9.943369999999998</v>
+      </c>
+      <c r="U61">
+        <f t="shared" si="6"/>
+        <v>8.7014000000000014</v>
+      </c>
+      <c r="V61">
+        <f t="shared" si="6"/>
+        <v>10.17971</v>
+      </c>
+      <c r="W61">
+        <f t="shared" si="6"/>
+        <v>6.2304720000000016</v>
+      </c>
+      <c r="X61">
+        <f t="shared" si="6"/>
+        <v>6.5973010000000016</v>
+      </c>
+      <c r="Y61">
+        <f t="shared" si="6"/>
+        <v>6.5830500000000001</v>
+      </c>
+      <c r="Z61">
+        <f t="shared" si="6"/>
+        <v>7.1959999999999997</v>
+      </c>
+      <c r="AA61">
+        <f t="shared" si="6"/>
+        <v>6.1785629999999996</v>
+      </c>
+      <c r="AB61">
+        <f t="shared" si="6"/>
+        <v>5.688771</v>
+      </c>
+      <c r="AC61">
+        <f t="shared" si="6"/>
+        <v>6.7748300000000006</v>
+      </c>
+      <c r="AD61">
+        <f t="shared" si="6"/>
+        <v>6.6588049999999992</v>
+      </c>
+      <c r="AE61">
+        <f t="shared" si="6"/>
+        <v>5.128855999999999</v>
+      </c>
+      <c r="AF61">
+        <f t="shared" si="6"/>
+        <v>5.5950500000000005</v>
+      </c>
+      <c r="AG61">
+        <f t="shared" si="6"/>
+        <v>3.917548</v>
+      </c>
+      <c r="AH61">
+        <f t="shared" si="6"/>
+        <v>4.8837099999999998</v>
+      </c>
+      <c r="AI61">
+        <f t="shared" si="6"/>
+        <v>5.3016700000000005</v>
+      </c>
+      <c r="AJ61">
+        <f t="shared" si="6"/>
+        <v>4.6582879999999998</v>
+      </c>
+      <c r="AK61">
+        <f t="shared" si="6"/>
+        <v>4.1578149999999994</v>
+      </c>
+      <c r="AL61">
+        <f t="shared" si="6"/>
+        <v>5.0510139999999994</v>
+      </c>
+      <c r="AM61">
+        <f t="shared" si="6"/>
+        <v>5.1072699999999998</v>
+      </c>
+      <c r="AN61">
+        <f t="shared" si="6"/>
+        <v>5.8146799999999992</v>
+      </c>
+      <c r="AO61">
+        <f t="shared" si="6"/>
+        <v>7.9684600000000003</v>
+      </c>
+      <c r="AP61">
+        <f t="shared" si="6"/>
+        <v>7.5288099999999991</v>
+      </c>
+      <c r="AQ61">
+        <f t="shared" si="6"/>
+        <v>10.96482</v>
+      </c>
+      <c r="AR61">
+        <f t="shared" si="6"/>
+        <v>7.0962679999999994</v>
+      </c>
+      <c r="AS61">
+        <f t="shared" si="6"/>
+        <v>7.323061</v>
+      </c>
+      <c r="AT61">
+        <f t="shared" si="6"/>
+        <v>8.8675499999999996</v>
+      </c>
+      <c r="AU61">
+        <f t="shared" si="6"/>
+        <v>8.7172299999999989</v>
+      </c>
+      <c r="AV61">
+        <f t="shared" si="6"/>
+        <v>13.878360000000002</v>
+      </c>
+      <c r="AW61">
+        <f t="shared" si="6"/>
+        <v>8.9170000000000016</v>
+      </c>
+      <c r="AX61">
+        <f t="shared" si="6"/>
+        <v>10.794740000000001</v>
+      </c>
+      <c r="AZ61">
+        <f t="shared" ref="AZ61:BB61" si="7">SUM(AZ4,AZ15:AZ16,AZ33,AZ35,AZ37:AZ38,AZ40,AZ55)</f>
+        <v>5.1158823636363646</v>
+      </c>
+      <c r="BA61">
+        <f t="shared" si="7"/>
+        <v>30.761986021238695</v>
+      </c>
+      <c r="BB61">
+        <f t="shared" si="7"/>
+        <v>76.96141636363636</v>
+      </c>
+    </row>
+    <row r="62" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="I62" t="s">
+        <v>73</v>
+      </c>
+      <c r="J62">
+        <f>SUM(J21:J23)</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="K62">
+        <f t="shared" ref="K62:AX62" si="8">SUM(K21:K23)</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="L62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="M62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="N62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="O62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="P62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="Q62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="R62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="S62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="T62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="U62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="V62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="W62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="X62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="Y62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="Z62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AA62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AB62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AC62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AD62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AE62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AF62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AG62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AH62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AI62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AJ62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AK62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AL62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AM62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AN62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AO62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AP62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AQ62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AR62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AS62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AT62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AU62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AV62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AW62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AX62">
+        <f t="shared" si="8"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AZ62">
+        <f t="shared" ref="AZ62:BB62" si="9">SUM(AZ21:AZ23)</f>
+        <v>0.6</v>
+      </c>
+      <c r="BA62">
+        <f t="shared" si="9"/>
+        <v>0.19226024346555501</v>
+      </c>
+      <c r="BB62">
+        <f t="shared" si="9"/>
+        <v>302.01</v>
+      </c>
+    </row>
+    <row r="63" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="AZ63">
+        <f>AZ60+AZ61+AZ62</f>
+        <v>26.874449745454548</v>
+      </c>
+    </row>
+    <row r="64" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="AZ64">
+        <f>SUM(AZ2:AZ56)</f>
+        <v>26.874449745454548</v>
       </c>
     </row>
   </sheetData>
@@ -13390,10 +14485,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB57"/>
+  <dimension ref="A1:BB64"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:I56"/>
+    <sheetView topLeftCell="A17" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60:BB64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21910,6 +23005,561 @@
       </c>
       <c r="AY57">
         <v>-999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="I60" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="J60">
+        <f>SUM(J2:J3,J5:J14,J17:J20,J24:J32,J34,J36,J39,J41:J54,J56)</f>
+        <v>463.66495000000009</v>
+      </c>
+      <c r="K60">
+        <f t="shared" ref="K60:AX60" si="4">SUM(K2:K3,K5:K14,K17:K20,K24:K32,K34,K36,K39,K41:K54,K56)</f>
+        <v>526.22991999999988</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="4"/>
+        <v>511.86675999999994</v>
+      </c>
+      <c r="M60">
+        <f t="shared" si="4"/>
+        <v>532.93748999999991</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="4"/>
+        <v>538.50757999999985</v>
+      </c>
+      <c r="O60">
+        <f t="shared" si="4"/>
+        <v>445.53336000000002</v>
+      </c>
+      <c r="P60">
+        <f t="shared" si="4"/>
+        <v>518.06934000000024</v>
+      </c>
+      <c r="Q60">
+        <f t="shared" si="4"/>
+        <v>456.90069999999986</v>
+      </c>
+      <c r="R60">
+        <f t="shared" si="4"/>
+        <v>445.90135999999995</v>
+      </c>
+      <c r="S60">
+        <f t="shared" si="4"/>
+        <v>430.87465000000009</v>
+      </c>
+      <c r="T60">
+        <f t="shared" si="4"/>
+        <v>344.95290999999997</v>
+      </c>
+      <c r="U60">
+        <f t="shared" si="4"/>
+        <v>465.73329999999999</v>
+      </c>
+      <c r="V60">
+        <f t="shared" si="4"/>
+        <v>418.88375000000025</v>
+      </c>
+      <c r="W60">
+        <f t="shared" si="4"/>
+        <v>448.32472999999999</v>
+      </c>
+      <c r="X60">
+        <f t="shared" si="4"/>
+        <v>502.93579000000011</v>
+      </c>
+      <c r="Y60">
+        <f t="shared" si="4"/>
+        <v>449.74839999999989</v>
+      </c>
+      <c r="Z60">
+        <f t="shared" si="4"/>
+        <v>502.10563000000002</v>
+      </c>
+      <c r="AA60">
+        <f t="shared" si="4"/>
+        <v>381.12975000000012</v>
+      </c>
+      <c r="AB60">
+        <f t="shared" si="4"/>
+        <v>461.94981999999987</v>
+      </c>
+      <c r="AC60">
+        <f t="shared" si="4"/>
+        <v>463.30757999999992</v>
+      </c>
+      <c r="AD60">
+        <f t="shared" si="4"/>
+        <v>499.81575000000004</v>
+      </c>
+      <c r="AE60">
+        <f t="shared" si="4"/>
+        <v>437.14291000000003</v>
+      </c>
+      <c r="AF60">
+        <f t="shared" si="4"/>
+        <v>543.82229000000007</v>
+      </c>
+      <c r="AG60">
+        <f t="shared" si="4"/>
+        <v>471.76654000000002</v>
+      </c>
+      <c r="AH60">
+        <f t="shared" si="4"/>
+        <v>470.0687099999999</v>
+      </c>
+      <c r="AI60">
+        <f t="shared" si="4"/>
+        <v>443.74534</v>
+      </c>
+      <c r="AJ60">
+        <f t="shared" si="4"/>
+        <v>409.52943000000005</v>
+      </c>
+      <c r="AK60">
+        <f t="shared" si="4"/>
+        <v>453.73378000000008</v>
+      </c>
+      <c r="AL60">
+        <f t="shared" si="4"/>
+        <v>530.15530000000001</v>
+      </c>
+      <c r="AM60">
+        <f t="shared" si="4"/>
+        <v>531.47502999999995</v>
+      </c>
+      <c r="AN60">
+        <f t="shared" si="4"/>
+        <v>468.63150000000007</v>
+      </c>
+      <c r="AO60">
+        <f t="shared" si="4"/>
+        <v>412.24232999999992</v>
+      </c>
+      <c r="AP60">
+        <f t="shared" si="4"/>
+        <v>451.12056000000001</v>
+      </c>
+      <c r="AQ60">
+        <f t="shared" si="4"/>
+        <v>519.64803999999992</v>
+      </c>
+      <c r="AR60">
+        <f t="shared" si="4"/>
+        <v>461.25547000000006</v>
+      </c>
+      <c r="AS60">
+        <f t="shared" si="4"/>
+        <v>432.38400000000001</v>
+      </c>
+      <c r="AT60">
+        <f t="shared" si="4"/>
+        <v>454.02517</v>
+      </c>
+      <c r="AU60">
+        <f t="shared" si="4"/>
+        <v>536.23517000000027</v>
+      </c>
+      <c r="AV60">
+        <f t="shared" si="4"/>
+        <v>542.5688600000002</v>
+      </c>
+      <c r="AW60">
+        <f t="shared" si="4"/>
+        <v>556.36981999999978</v>
+      </c>
+      <c r="AX60">
+        <f t="shared" si="4"/>
+        <v>518.57441999999992</v>
+      </c>
+      <c r="AZ60">
+        <f t="shared" ref="AZ60:BB60" si="5">SUM(AZ2:AZ3,AZ5:AZ14,AZ17:AZ20,AZ24:AZ32,AZ34,AZ36,AZ39,AZ41:AZ54,AZ56)</f>
+        <v>478.17150727272735</v>
+      </c>
+      <c r="BA60">
+        <f t="shared" si="5"/>
+        <v>5948.2151775372795</v>
+      </c>
+      <c r="BB60">
+        <f t="shared" si="5"/>
+        <v>198.85098909090908</v>
+      </c>
+    </row>
+    <row r="61" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="I61" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="J61">
+        <f>SUM(J4,J15:J16,J33,J35,J37:J38,J40,J55)</f>
+        <v>154.59210000000002</v>
+      </c>
+      <c r="K61">
+        <f t="shared" ref="K61:AX61" si="6">SUM(K4,K15:K16,K33,K35,K37:K38,K40,K55)</f>
+        <v>165.89440000000002</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="6"/>
+        <v>175.94419999999997</v>
+      </c>
+      <c r="M61">
+        <f t="shared" si="6"/>
+        <v>182.57199999999997</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="6"/>
+        <v>181.29279999999997</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="6"/>
+        <v>185.98400000000004</v>
+      </c>
+      <c r="P61">
+        <f t="shared" si="6"/>
+        <v>170.96139999999997</v>
+      </c>
+      <c r="Q61">
+        <f t="shared" si="6"/>
+        <v>165.98240000000001</v>
+      </c>
+      <c r="R61">
+        <f t="shared" si="6"/>
+        <v>190.38220000000001</v>
+      </c>
+      <c r="S61">
+        <f t="shared" si="6"/>
+        <v>122.00995000000002</v>
+      </c>
+      <c r="T61">
+        <f t="shared" si="6"/>
+        <v>121.98010000000002</v>
+      </c>
+      <c r="U61">
+        <f t="shared" si="6"/>
+        <v>150.94539999999998</v>
+      </c>
+      <c r="V61">
+        <f t="shared" si="6"/>
+        <v>180.37230000000002</v>
+      </c>
+      <c r="W61">
+        <f t="shared" si="6"/>
+        <v>159.75279999999998</v>
+      </c>
+      <c r="X61">
+        <f t="shared" si="6"/>
+        <v>181.49099999999999</v>
+      </c>
+      <c r="Y61">
+        <f t="shared" si="6"/>
+        <v>161.80290000000002</v>
+      </c>
+      <c r="Z61">
+        <f t="shared" si="6"/>
+        <v>170.82330000000002</v>
+      </c>
+      <c r="AA61">
+        <f t="shared" si="6"/>
+        <v>162.67359999999999</v>
+      </c>
+      <c r="AB61">
+        <f t="shared" si="6"/>
+        <v>142.83110000000002</v>
+      </c>
+      <c r="AC61">
+        <f t="shared" si="6"/>
+        <v>164.90260000000001</v>
+      </c>
+      <c r="AD61">
+        <f t="shared" si="6"/>
+        <v>171.8759</v>
+      </c>
+      <c r="AE61">
+        <f t="shared" si="6"/>
+        <v>164.30470000000005</v>
+      </c>
+      <c r="AF61">
+        <f t="shared" si="6"/>
+        <v>131.90570000000002</v>
+      </c>
+      <c r="AG61">
+        <f t="shared" si="6"/>
+        <v>116.58159999999998</v>
+      </c>
+      <c r="AH61">
+        <f t="shared" si="6"/>
+        <v>149.74909999999997</v>
+      </c>
+      <c r="AI61">
+        <f t="shared" si="6"/>
+        <v>140.65279999999998</v>
+      </c>
+      <c r="AJ61">
+        <f t="shared" si="6"/>
+        <v>148.00206</v>
+      </c>
+      <c r="AK61">
+        <f t="shared" si="6"/>
+        <v>127.51130000000001</v>
+      </c>
+      <c r="AL61">
+        <f t="shared" si="6"/>
+        <v>139.36220000000003</v>
+      </c>
+      <c r="AM61">
+        <f t="shared" si="6"/>
+        <v>130.25450000000001</v>
+      </c>
+      <c r="AN61">
+        <f t="shared" si="6"/>
+        <v>155.07830000000001</v>
+      </c>
+      <c r="AO61">
+        <f t="shared" si="6"/>
+        <v>135.24480000000003</v>
+      </c>
+      <c r="AP61">
+        <f t="shared" si="6"/>
+        <v>125.88990000000001</v>
+      </c>
+      <c r="AQ61">
+        <f t="shared" si="6"/>
+        <v>166.92139999999998</v>
+      </c>
+      <c r="AR61">
+        <f t="shared" si="6"/>
+        <v>120.7075</v>
+      </c>
+      <c r="AS61">
+        <f t="shared" si="6"/>
+        <v>125.48150000000004</v>
+      </c>
+      <c r="AT61">
+        <f t="shared" si="6"/>
+        <v>145.42850000000001</v>
+      </c>
+      <c r="AU61">
+        <f t="shared" si="6"/>
+        <v>145.9093</v>
+      </c>
+      <c r="AV61">
+        <f t="shared" si="6"/>
+        <v>209.73080000000002</v>
+      </c>
+      <c r="AW61">
+        <f t="shared" si="6"/>
+        <v>150.91550000000001</v>
+      </c>
+      <c r="AX61">
+        <f t="shared" si="6"/>
+        <v>172.18900000000002</v>
+      </c>
+      <c r="AZ61">
+        <f t="shared" ref="AZ61:BB61" si="7">SUM(AZ4,AZ15:AZ16,AZ33,AZ35,AZ37:AZ38,AZ40,AZ55)</f>
+        <v>143.20710545454546</v>
+      </c>
+      <c r="BA61">
+        <f t="shared" si="7"/>
+        <v>1539.5253614831154</v>
+      </c>
+      <c r="BB61">
+        <f t="shared" si="7"/>
+        <v>76.96141636363636</v>
+      </c>
+    </row>
+    <row r="62" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="I62" t="s">
+        <v>73</v>
+      </c>
+      <c r="J62">
+        <f>SUM(J21:J23)</f>
+        <v>39</v>
+      </c>
+      <c r="K62">
+        <f t="shared" ref="K62:AX62" si="8">SUM(K21:K23)</f>
+        <v>39</v>
+      </c>
+      <c r="L62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="M62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="N62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="O62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="P62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="Q62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="R62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="S62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="T62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="U62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="V62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="W62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="X62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="Y62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="Z62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="AA62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="AB62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="AC62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="AD62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="AE62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="AF62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="AG62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="AH62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="AI62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="AJ62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="AK62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="AL62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="AM62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="AN62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="AO62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="AP62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="AQ62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="AR62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="AS62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="AT62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="AU62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="AV62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="AW62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="AX62">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="AZ62">
+        <f t="shared" ref="AZ62:BB62" si="9">SUM(AZ21:AZ23)</f>
+        <v>39</v>
+      </c>
+      <c r="BA62">
+        <f t="shared" si="9"/>
+        <v>27.67174218450667</v>
+      </c>
+      <c r="BB62">
+        <f t="shared" si="9"/>
+        <v>302.01</v>
+      </c>
+    </row>
+    <row r="63" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="AZ63">
+        <f>AZ60+AZ61+AZ62</f>
+        <v>660.37861272727287</v>
+      </c>
+    </row>
+    <row r="64" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="AZ64">
+        <f>SUM(AZ2:AZ56)</f>
+        <v>660.37861272727264</v>
       </c>
     </row>
   </sheetData>
@@ -21920,10 +23570,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB62"/>
+  <dimension ref="A1:BB64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:AX20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -25713,179 +27363,179 @@
         <v>238</v>
       </c>
       <c r="J21">
-        <f>KM3perYR_NOBLS!J21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!J21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="K21">
-        <f>KM3perYR_NOBLS!K21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!K21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="L21">
-        <f>KM3perYR_NOBLS!L21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!L21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="M21">
-        <f>KM3perYR_NOBLS!M21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!M21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="N21">
-        <f>KM3perYR_NOBLS!N21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!N21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="O21">
-        <f>KM3perYR_NOBLS!O21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!O21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="P21">
-        <f>KM3perYR_NOBLS!P21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!P21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="Q21">
-        <f>KM3perYR_NOBLS!Q21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!Q21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="R21">
-        <f>KM3perYR_NOBLS!R21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!R21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="S21">
-        <f>KM3perYR_NOBLS!S21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!S21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="T21">
-        <f>KM3perYR_NOBLS!T21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!T21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="U21">
-        <f>KM3perYR_NOBLS!U21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!U21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="V21">
-        <f>KM3perYR_NOBLS!V21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!V21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="W21">
-        <f>KM3perYR_NOBLS!W21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!W21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="X21">
-        <f>KM3perYR_NOBLS!X21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!X21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="Y21">
-        <f>KM3perYR_NOBLS!Y21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!Y21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="Z21">
-        <f>KM3perYR_NOBLS!Z21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!Z21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AA21">
-        <f>KM3perYR_NOBLS!AA21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AA21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AB21">
-        <f>KM3perYR_NOBLS!AB21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AB21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AC21">
-        <f>KM3perYR_NOBLS!AC21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AC21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AD21">
-        <f>KM3perYR_NOBLS!AD21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AD21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AE21">
-        <f>KM3perYR_NOBLS!AE21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AE21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AF21">
-        <f>KM3perYR_NOBLS!AF21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AF21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AG21">
-        <f>KM3perYR_NOBLS!AG21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AG21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AH21">
-        <f>KM3perYR_NOBLS!AH21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AH21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AI21">
-        <f>KM3perYR_NOBLS!AI21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AI21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AJ21">
-        <f>KM3perYR_NOBLS!AJ21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AJ21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AK21">
-        <f>KM3perYR_NOBLS!AK21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AK21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AL21">
-        <f>KM3perYR_NOBLS!AL21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AL21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AM21">
-        <f>KM3perYR_NOBLS!AM21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AM21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AN21">
-        <f>KM3perYR_NOBLS!AN21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AN21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AO21">
-        <f>KM3perYR_NOBLS!AO21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AO21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AP21">
-        <f>KM3perYR_NOBLS!AP21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AP21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AQ21">
-        <f>KM3perYR_NOBLS!AQ21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AQ21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AR21">
-        <f>KM3perYR_NOBLS!AR21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AR21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AS21">
-        <f>KM3perYR_NOBLS!AS21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AS21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AT21">
-        <f>KM3perYR_NOBLS!AT21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AT21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AU21">
-        <f>KM3perYR_NOBLS!AU21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AU21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AV21">
-        <f>KM3perYR_NOBLS!AV21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AV21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AW21">
-        <f>KM3perYR_NOBLS!AW21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AW21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AX21">
-        <f>KM3perYR_NOBLS!AX21*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AX21*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AY21">
         <v>-999</v>
       </c>
       <c r="AZ21">
         <f t="shared" si="2"/>
-        <v>5.6548352399999979</v>
+        <v>7.0469000000000017</v>
       </c>
       <c r="BA21">
         <f t="shared" si="3"/>
-        <v>2.0061428571428563</v>
+        <v>2.5000000000000004</v>
       </c>
       <c r="BB21">
         <f>KM3perYR_NOBLS!AZ21</f>
@@ -25903,179 +27553,179 @@
         <v>237</v>
       </c>
       <c r="J22">
-        <f>KM3perYR_NOBLS!J22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!J22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="K22">
-        <f>KM3perYR_NOBLS!K22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!K22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="L22">
-        <f>KM3perYR_NOBLS!L22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!L22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="M22">
-        <f>KM3perYR_NOBLS!M22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!M22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="N22">
-        <f>KM3perYR_NOBLS!N22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!N22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="O22">
-        <f>KM3perYR_NOBLS!O22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!O22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="P22">
-        <f>KM3perYR_NOBLS!P22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!P22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="Q22">
-        <f>KM3perYR_NOBLS!Q22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!Q22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="R22">
-        <f>KM3perYR_NOBLS!R22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!R22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="S22">
-        <f>KM3perYR_NOBLS!S22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!S22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="T22">
-        <f>KM3perYR_NOBLS!T22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!T22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="U22">
-        <f>KM3perYR_NOBLS!U22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!U22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="V22">
-        <f>KM3perYR_NOBLS!V22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!V22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="W22">
-        <f>KM3perYR_NOBLS!W22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!W22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="X22">
-        <f>KM3perYR_NOBLS!X22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!X22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="Y22">
-        <f>KM3perYR_NOBLS!Y22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!Y22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="Z22">
-        <f>KM3perYR_NOBLS!Z22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!Z22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AA22">
-        <f>KM3perYR_NOBLS!AA22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AA22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AB22">
-        <f>KM3perYR_NOBLS!AB22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AB22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AC22">
-        <f>KM3perYR_NOBLS!AC22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AC22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AD22">
-        <f>KM3perYR_NOBLS!AD22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AD22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AE22">
-        <f>KM3perYR_NOBLS!AE22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AE22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AF22">
-        <f>KM3perYR_NOBLS!AF22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AF22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AG22">
-        <f>KM3perYR_NOBLS!AG22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AG22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AH22">
-        <f>KM3perYR_NOBLS!AH22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AH22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AI22">
-        <f>KM3perYR_NOBLS!AI22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AI22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AJ22">
-        <f>KM3perYR_NOBLS!AJ22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AJ22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AK22">
-        <f>KM3perYR_NOBLS!AK22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AK22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AL22">
-        <f>KM3perYR_NOBLS!AL22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AL22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AM22">
-        <f>KM3perYR_NOBLS!AM22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AM22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AN22">
-        <f>KM3perYR_NOBLS!AN22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AN22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AO22">
-        <f>KM3perYR_NOBLS!AO22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AO22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AP22">
-        <f>KM3perYR_NOBLS!AP22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AP22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AQ22">
-        <f>KM3perYR_NOBLS!AQ22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AQ22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AR22">
-        <f>KM3perYR_NOBLS!AR22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AR22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AS22">
-        <f>KM3perYR_NOBLS!AS22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AS22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AT22">
-        <f>KM3perYR_NOBLS!AT22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AT22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AU22">
-        <f>KM3perYR_NOBLS!AU22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AU22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AV22">
-        <f>KM3perYR_NOBLS!AV22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AV22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AW22">
-        <f>KM3perYR_NOBLS!AW22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AW22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AX22">
-        <f>KM3perYR_NOBLS!AX22*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AX22*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AY22">
         <v>-999</v>
       </c>
       <c r="AZ22">
         <f t="shared" si="2"/>
-        <v>5.6548352399999979</v>
+        <v>7.0469000000000017</v>
       </c>
       <c r="BA22">
         <f t="shared" si="3"/>
-        <v>2.0061428571428563</v>
+        <v>2.5000000000000004</v>
       </c>
       <c r="BB22">
         <f>KM3perYR_NOBLS!AZ22</f>
@@ -26093,179 +27743,179 @@
         <v>236</v>
       </c>
       <c r="J23">
-        <f>KM3perYR_NOBLS!J23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!J23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="K23">
-        <f>KM3perYR_NOBLS!K23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!K23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="L23">
-        <f>KM3perYR_NOBLS!L23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!L23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="M23">
-        <f>KM3perYR_NOBLS!M23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!M23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="N23">
-        <f>KM3perYR_NOBLS!N23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!N23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="O23">
-        <f>KM3perYR_NOBLS!O23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!O23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="P23">
-        <f>KM3perYR_NOBLS!P23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!P23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="Q23">
-        <f>KM3perYR_NOBLS!Q23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!Q23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="R23">
-        <f>KM3perYR_NOBLS!R23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!R23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="S23">
-        <f>KM3perYR_NOBLS!S23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!S23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="T23">
-        <f>KM3perYR_NOBLS!T23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!T23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="U23">
-        <f>KM3perYR_NOBLS!U23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!U23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="V23">
-        <f>KM3perYR_NOBLS!V23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!V23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="W23">
-        <f>KM3perYR_NOBLS!W23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!W23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="X23">
-        <f>KM3perYR_NOBLS!X23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!X23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="Y23">
-        <f>KM3perYR_NOBLS!Y23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!Y23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="Z23">
-        <f>KM3perYR_NOBLS!Z23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!Z23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AA23">
-        <f>KM3perYR_NOBLS!AA23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AA23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AB23">
-        <f>KM3perYR_NOBLS!AB23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AB23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AC23">
-        <f>KM3perYR_NOBLS!AC23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AC23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AD23">
-        <f>KM3perYR_NOBLS!AD23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AD23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AE23">
-        <f>KM3perYR_NOBLS!AE23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AE23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AF23">
-        <f>KM3perYR_NOBLS!AF23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AF23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AG23">
-        <f>KM3perYR_NOBLS!AG23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AG23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AH23">
-        <f>KM3perYR_NOBLS!AH23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AH23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AI23">
-        <f>KM3perYR_NOBLS!AI23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AI23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AJ23">
-        <f>KM3perYR_NOBLS!AJ23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AJ23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AK23">
-        <f>KM3perYR_NOBLS!AK23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AK23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AL23">
-        <f>KM3perYR_NOBLS!AL23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AL23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AM23">
-        <f>KM3perYR_NOBLS!AM23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AM23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AN23">
-        <f>KM3perYR_NOBLS!AN23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AN23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AO23">
-        <f>KM3perYR_NOBLS!AO23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AO23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AP23">
-        <f>KM3perYR_NOBLS!AP23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AP23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AQ23">
-        <f>KM3perYR_NOBLS!AQ23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AQ23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AR23">
-        <f>KM3perYR_NOBLS!AR23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AR23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AS23">
-        <f>KM3perYR_NOBLS!AS23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AS23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AT23">
-        <f>KM3perYR_NOBLS!AT23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AT23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AU23">
-        <f>KM3perYR_NOBLS!AU23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AU23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AV23">
-        <f>KM3perYR_NOBLS!AV23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AV23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AW23">
-        <f>KM3perYR_NOBLS!AW23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AW23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AX23">
-        <f>KM3perYR_NOBLS!AX23*0.056172</f>
-        <v>5.6548352399999997</v>
+        <f>KM3perYR_NOBLS!AX23*0.07</f>
+        <v>7.0469000000000008</v>
       </c>
       <c r="AY23">
         <v>-999</v>
       </c>
       <c r="AZ23">
         <f t="shared" si="2"/>
-        <v>5.6548352399999979</v>
+        <v>7.0469000000000017</v>
       </c>
       <c r="BA23">
         <f t="shared" si="3"/>
-        <v>2.0061428571428563</v>
+        <v>2.5000000000000004</v>
       </c>
       <c r="BB23">
         <f>KM3perYR_NOBLS!AZ23</f>
@@ -32710,54 +34360,559 @@
       </c>
     </row>
     <row r="60" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="J60" s="4"/>
-      <c r="K60" s="4"/>
-      <c r="L60" s="4"/>
-      <c r="M60" s="4"/>
-      <c r="N60" s="4"/>
-      <c r="O60" s="4"/>
-      <c r="P60" s="4"/>
-      <c r="Q60" s="4"/>
-      <c r="R60" s="4"/>
-      <c r="S60" s="4"/>
-      <c r="T60" s="4"/>
-      <c r="U60" s="4"/>
-      <c r="V60" s="4"/>
-      <c r="W60" s="4"/>
-      <c r="X60" s="4"/>
-      <c r="Y60" s="4"/>
-      <c r="Z60" s="4"/>
-      <c r="AA60" s="4"/>
-      <c r="AB60" s="4"/>
-      <c r="AC60" s="4"/>
-      <c r="AD60" s="4"/>
+      <c r="I60" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="J60">
+        <f>SUM(J2:J3,J5:J14,J17:J20,J24:J32,J34,J36,J39,J41:J54,J56)</f>
+        <v>1069.0068800000001</v>
+      </c>
+      <c r="K60">
+        <f t="shared" ref="K60:AX60" si="4">SUM(K2:K3,K5:K14,K17:K20,K24:K32,K34,K36,K39,K41:K54,K56)</f>
+        <v>921.91628000000003</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="4"/>
+        <v>849.18375999999989</v>
+      </c>
+      <c r="M60">
+        <f t="shared" si="4"/>
+        <v>1050.9931600000002</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="4"/>
+        <v>1086.4139600000001</v>
+      </c>
+      <c r="O60">
+        <f t="shared" si="4"/>
+        <v>856.0052800000002</v>
+      </c>
+      <c r="P60">
+        <f t="shared" si="4"/>
+        <v>1029.5030399999998</v>
+      </c>
+      <c r="Q60">
+        <f t="shared" si="4"/>
+        <v>795.78307999999981</v>
+      </c>
+      <c r="R60">
+        <f t="shared" si="4"/>
+        <v>734.44327999999996</v>
+      </c>
+      <c r="S60">
+        <f t="shared" si="4"/>
+        <v>755.46212000000014</v>
+      </c>
+      <c r="T60">
+        <f t="shared" si="4"/>
+        <v>498.84392000000008</v>
+      </c>
+      <c r="U60">
+        <f t="shared" si="4"/>
+        <v>969.47328000000005</v>
+      </c>
+      <c r="V60">
+        <f t="shared" si="4"/>
+        <v>752.23712</v>
+      </c>
+      <c r="W60">
+        <f t="shared" si="4"/>
+        <v>834.87648000000013</v>
+      </c>
+      <c r="X60">
+        <f t="shared" si="4"/>
+        <v>1002.6108799999998</v>
+      </c>
+      <c r="Y60">
+        <f t="shared" si="4"/>
+        <v>865.4646799999997</v>
+      </c>
+      <c r="Z60">
+        <f t="shared" si="4"/>
+        <v>863.71695999999997</v>
+      </c>
+      <c r="AA60">
+        <f t="shared" si="4"/>
+        <v>581.04548</v>
+      </c>
+      <c r="AB60">
+        <f t="shared" si="4"/>
+        <v>909.47052000000019</v>
+      </c>
+      <c r="AC60">
+        <f t="shared" si="4"/>
+        <v>798.60195999999996</v>
+      </c>
+      <c r="AD60">
+        <f t="shared" si="4"/>
+        <v>860.80787999999973</v>
+      </c>
+      <c r="AE60">
+        <f t="shared" si="4"/>
+        <v>715.90787999999986</v>
+      </c>
+      <c r="AF60">
+        <f t="shared" si="4"/>
+        <v>856.92800000000011</v>
+      </c>
+      <c r="AG60">
+        <f t="shared" si="4"/>
+        <v>767.61120000000005</v>
+      </c>
+      <c r="AH60">
+        <f t="shared" si="4"/>
+        <v>765.45963999999981</v>
+      </c>
+      <c r="AI60">
+        <f t="shared" si="4"/>
+        <v>744.01376000000005</v>
+      </c>
+      <c r="AJ60">
+        <f t="shared" si="4"/>
+        <v>545.59616000000005</v>
+      </c>
+      <c r="AK60">
+        <f t="shared" si="4"/>
+        <v>775.44699999999978</v>
+      </c>
+      <c r="AL60">
+        <f t="shared" si="4"/>
+        <v>929.08487999999988</v>
+      </c>
+      <c r="AM60">
+        <f t="shared" si="4"/>
+        <v>930.20912000000021</v>
+      </c>
+      <c r="AN60">
+        <f t="shared" si="4"/>
+        <v>858.37800000000004</v>
+      </c>
+      <c r="AO60">
+        <f t="shared" si="4"/>
+        <v>529.91411999999991</v>
+      </c>
+      <c r="AP60">
+        <f t="shared" si="4"/>
+        <v>728.42876000000024</v>
+      </c>
+      <c r="AQ60">
+        <f t="shared" si="4"/>
+        <v>942.7732400000001</v>
+      </c>
+      <c r="AR60">
+        <f t="shared" si="4"/>
+        <v>645.84656000000007</v>
+      </c>
+      <c r="AS60">
+        <f t="shared" si="4"/>
+        <v>535.53516000000002</v>
+      </c>
+      <c r="AT60">
+        <f t="shared" si="4"/>
+        <v>738.96119999999985</v>
+      </c>
+      <c r="AU60">
+        <f t="shared" si="4"/>
+        <v>1042.4766000000002</v>
+      </c>
+      <c r="AV60">
+        <f t="shared" si="4"/>
+        <v>998.15840000000014</v>
+      </c>
+      <c r="AW60">
+        <f t="shared" si="4"/>
+        <v>1061.8543999999997</v>
+      </c>
+      <c r="AX60">
+        <f t="shared" si="4"/>
+        <v>888.21252000000015</v>
+      </c>
       <c r="AZ60">
-        <f>SUM(AZ2:AZ56)</f>
-        <v>1120.2141275381816</v>
+        <f t="shared" ref="AZ60:BB60" si="5">SUM(AZ2:AZ3,AZ5:AZ14,AZ17:AZ20,AZ24:AZ32,AZ34,AZ36,AZ39,AZ41:AZ54,AZ56)</f>
+        <v>795.40395636363633</v>
+      </c>
+      <c r="BA60">
+        <f t="shared" si="5"/>
+        <v>6142.857142857144</v>
+      </c>
+      <c r="BB60">
+        <f t="shared" si="5"/>
+        <v>198.85098909090908</v>
+      </c>
+    </row>
+    <row r="61" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="I61" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="J61">
+        <f>SUM(J4,J15:J16,J33,J35,J37:J38,J40,J55)</f>
+        <v>370.10519999999997</v>
+      </c>
+      <c r="K61">
+        <f t="shared" ref="K61:AX61" si="6">SUM(K4,K15:K16,K33,K35,K37:K38,K40,K55)</f>
+        <v>360.78960000000001</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="6"/>
+        <v>364.30480000000006</v>
+      </c>
+      <c r="M61">
+        <f t="shared" si="6"/>
+        <v>375.44000000000005</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="6"/>
+        <v>361.16719999999998</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="6"/>
+        <v>355.96840000000003</v>
+      </c>
+      <c r="P61">
+        <f t="shared" si="6"/>
+        <v>340.178</v>
+      </c>
+      <c r="Q61">
+        <f t="shared" si="6"/>
+        <v>349.56800000000004</v>
+      </c>
+      <c r="R61">
+        <f t="shared" si="6"/>
+        <v>391.5444</v>
+      </c>
+      <c r="S61">
+        <f t="shared" si="6"/>
+        <v>221.58507999999995</v>
+      </c>
+      <c r="T61">
+        <f t="shared" si="6"/>
+        <v>239.08295999999996</v>
+      </c>
+      <c r="U61">
+        <f t="shared" si="6"/>
+        <v>293.88832000000002</v>
+      </c>
+      <c r="V61">
+        <f t="shared" si="6"/>
+        <v>333.11760000000004</v>
+      </c>
+      <c r="W61">
+        <f t="shared" si="6"/>
+        <v>332.35039999999998</v>
+      </c>
+      <c r="X61">
+        <f t="shared" si="6"/>
+        <v>379.67039999999992</v>
+      </c>
+      <c r="Y61">
+        <f t="shared" si="6"/>
+        <v>352.9932</v>
+      </c>
+      <c r="Z61">
+        <f t="shared" si="6"/>
+        <v>355.14840000000004</v>
+      </c>
+      <c r="AA61">
+        <f t="shared" si="6"/>
+        <v>315.31920000000002</v>
+      </c>
+      <c r="AB61">
+        <f t="shared" si="6"/>
+        <v>280.86400000000003</v>
+      </c>
+      <c r="AC61">
+        <f t="shared" si="6"/>
+        <v>360.98320000000007</v>
+      </c>
+      <c r="AD61">
+        <f t="shared" si="6"/>
+        <v>330.52339999999998</v>
+      </c>
+      <c r="AE61">
+        <f t="shared" si="6"/>
+        <v>363.07360000000006</v>
+      </c>
+      <c r="AF61">
+        <f t="shared" si="6"/>
+        <v>296.16551999999996</v>
+      </c>
+      <c r="AG61">
+        <f t="shared" si="6"/>
+        <v>284.41371999999996</v>
+      </c>
+      <c r="AH61">
+        <f t="shared" si="6"/>
+        <v>291.04079999999999</v>
+      </c>
+      <c r="AI61">
+        <f t="shared" si="6"/>
+        <v>250.00519999999995</v>
+      </c>
+      <c r="AJ61">
+        <f t="shared" si="6"/>
+        <v>267.50736000000001</v>
+      </c>
+      <c r="AK61">
+        <f t="shared" si="6"/>
+        <v>286.63119999999998</v>
+      </c>
+      <c r="AL61">
+        <f t="shared" si="6"/>
+        <v>329.57311999999996</v>
+      </c>
+      <c r="AM61">
+        <f t="shared" si="6"/>
+        <v>303.78000000000003</v>
+      </c>
+      <c r="AN61">
+        <f t="shared" si="6"/>
+        <v>383.58839999999998</v>
+      </c>
+      <c r="AO61">
+        <f t="shared" si="6"/>
+        <v>289.80871999999999</v>
+      </c>
+      <c r="AP61">
+        <f t="shared" si="6"/>
+        <v>279.33999999999997</v>
+      </c>
+      <c r="AQ61">
+        <f t="shared" si="6"/>
+        <v>468.13800000000009</v>
+      </c>
+      <c r="AR61">
+        <f t="shared" si="6"/>
+        <v>239.41392000000002</v>
+      </c>
+      <c r="AS61">
+        <f t="shared" si="6"/>
+        <v>253.68619999999999</v>
+      </c>
+      <c r="AT61">
+        <f t="shared" si="6"/>
+        <v>326.62551999999999</v>
+      </c>
+      <c r="AU61">
+        <f t="shared" si="6"/>
+        <v>309.01599999999996</v>
+      </c>
+      <c r="AV61">
+        <f t="shared" si="6"/>
+        <v>585.33039999999994</v>
+      </c>
+      <c r="AW61">
+        <f t="shared" si="6"/>
+        <v>312.99399999999997</v>
+      </c>
+      <c r="AX61">
+        <f t="shared" si="6"/>
+        <v>397.56279999999998</v>
+      </c>
+      <c r="AZ61">
+        <f t="shared" ref="AZ61:BB61" si="7">SUM(AZ4,AZ15:AZ16,AZ33,AZ35,AZ37:AZ38,AZ40,AZ55)</f>
+        <v>307.84566545454544</v>
+      </c>
+      <c r="BA61">
+        <f t="shared" si="7"/>
+        <v>1285.7142857142858</v>
+      </c>
+      <c r="BB61">
+        <f t="shared" si="7"/>
+        <v>76.96141636363636</v>
       </c>
     </row>
     <row r="62" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="J62" s="4"/>
-      <c r="K62" s="4"/>
-      <c r="L62" s="4"/>
-      <c r="M62" s="4"/>
-      <c r="N62" s="4"/>
-      <c r="O62" s="4"/>
-      <c r="P62" s="4"/>
-      <c r="Q62" s="4"/>
-      <c r="R62" s="4"/>
-      <c r="S62" s="4"/>
-      <c r="T62" s="4"/>
-      <c r="U62" s="4"/>
-      <c r="V62" s="4"/>
-      <c r="W62" s="4"/>
-      <c r="X62" s="4"/>
-      <c r="Y62" s="4"/>
-      <c r="Z62" s="4"/>
-      <c r="AA62" s="4"/>
-      <c r="AB62" s="4"/>
-      <c r="AC62" s="4"/>
-      <c r="AD62" s="4"/>
+      <c r="I62" t="s">
+        <v>73</v>
+      </c>
+      <c r="J62">
+        <f>SUM(J21:J23)</f>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="K62">
+        <f t="shared" ref="K62:AX62" si="8">SUM(K21:K23)</f>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="L62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="M62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="N62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="O62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="P62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="Q62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="R62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="S62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="T62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="U62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="V62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="W62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="X62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="Y62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="Z62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="AA62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="AB62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="AC62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="AD62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="AE62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="AF62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="AG62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="AH62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="AI62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="AJ62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="AK62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="AL62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="AM62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="AN62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="AO62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="AP62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="AQ62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="AR62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="AS62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="AT62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="AU62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="AV62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="AW62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="AX62">
+        <f t="shared" si="8"/>
+        <v>21.140700000000002</v>
+      </c>
+      <c r="AZ62">
+        <f t="shared" ref="AZ62:BB62" si="9">SUM(AZ21:AZ23)</f>
+        <v>21.140700000000006</v>
+      </c>
+      <c r="BA62">
+        <f t="shared" si="9"/>
+        <v>7.5000000000000018</v>
+      </c>
+      <c r="BB62">
+        <f t="shared" si="9"/>
+        <v>302.01</v>
+      </c>
+    </row>
+    <row r="63" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="AZ63">
+        <f>AZ60+AZ61+AZ62</f>
+        <v>1124.3903218181817</v>
+      </c>
+    </row>
+    <row r="64" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="AZ64">
+        <f>SUM(AZ2:AZ56)</f>
+        <v>1124.3903218181817</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -32767,10 +34922,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB57"/>
+  <dimension ref="A1:BB65"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C56"/>
+    <sheetView topLeftCell="AM12" workbookViewId="0">
+      <selection activeCell="BB60" sqref="I60:BB66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -41287,6 +43442,567 @@
       </c>
       <c r="AY57">
         <v>-999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="I60" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="J60">
+        <f>SUM(J2:J3,J5:J14,J17:J20,J24:J32,J34,J36,J39,J41:J54,J56)</f>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="K60">
+        <f t="shared" ref="K60:AX60" si="4">SUM(K2:K3,K5:K14,K17:K20,K24:K32,K34,K36,K39,K41:K54,K56)</f>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="M60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="O60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="P60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="Q60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="R60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="S60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="T60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="U60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="V60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="W60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="X60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="Y60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="Z60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="AA60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="AB60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="AC60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="AD60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="AE60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="AF60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="AG60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="AH60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="AI60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="AJ60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="AK60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="AL60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="AM60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="AN60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="AO60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="AP60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="AQ60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="AR60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="AS60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="AT60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="AU60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="AV60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="AW60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="AX60">
+        <f t="shared" si="4"/>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="AZ60">
+        <f t="shared" ref="AZ60:BB60" si="5">SUM(AZ2:AZ3,AZ5:AZ14,AZ17:AZ20,AZ24:AZ32,AZ34,AZ36,AZ39,AZ41:AZ54,AZ56)</f>
+        <v>6539.5173999999997</v>
+      </c>
+      <c r="BA60">
+        <f t="shared" si="5"/>
+        <v>105643.31872861959</v>
+      </c>
+      <c r="BB60">
+        <f t="shared" si="5"/>
+        <v>198.85098909090908</v>
+      </c>
+    </row>
+    <row r="61" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="I61" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="J61">
+        <f>SUM(J4,J15:J16,J33,J35,J37:J38,J40,J55)</f>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="K61">
+        <f t="shared" ref="K61:AX61" si="6">SUM(K4,K15:K16,K33,K35,K37:K38,K40,K55)</f>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="M61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="P61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="Q61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="R61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="S61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="T61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="U61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="V61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="W61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="X61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="Y61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="Z61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="AA61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="AB61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="AC61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="AD61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="AE61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="AF61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="AG61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="AH61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="AI61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="AJ61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="AK61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="AL61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="AM61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="AN61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="AO61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="AP61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="AQ61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="AR61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="AS61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="AT61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="AU61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="AV61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="AW61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="AX61">
+        <f t="shared" si="6"/>
+        <v>2746.3960000000006</v>
+      </c>
+      <c r="AZ61">
+        <f t="shared" ref="AZ61:BB61" si="7">SUM(AZ4,AZ15:AZ16,AZ33,AZ35,AZ37:AZ38,AZ40,AZ55)</f>
+        <v>2746.3960000000011</v>
+      </c>
+      <c r="BA61">
+        <f t="shared" si="7"/>
+        <v>28565.781853707045</v>
+      </c>
+      <c r="BB61">
+        <f t="shared" si="7"/>
+        <v>76.96141636363636</v>
+      </c>
+    </row>
+    <row r="62" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="I62" t="s">
+        <v>73</v>
+      </c>
+      <c r="J62">
+        <f>SUM(J21:J23)</f>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="K62">
+        <f t="shared" ref="K62:AX62" si="8">SUM(K21:K23)</f>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="L62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="M62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="N62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="O62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="P62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="Q62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="R62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="S62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="T62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="U62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="V62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="W62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="X62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="Y62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="Z62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="AA62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="AB62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="AC62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="AD62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="AE62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="AF62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="AG62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="AH62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="AI62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="AJ62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="AK62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="AL62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="AM62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="AN62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="AO62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="AP62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="AQ62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="AR62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="AS62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="AT62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="AU62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="AV62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="AW62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="AX62">
+        <f t="shared" si="8"/>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="AZ62">
+        <f t="shared" ref="AZ62:BB62" si="9">SUM(AZ21:AZ23)</f>
+        <v>10091.400000000001</v>
+      </c>
+      <c r="BA62">
+        <f t="shared" si="9"/>
+        <v>7160.1697200187336</v>
+      </c>
+      <c r="BB62">
+        <f t="shared" si="9"/>
+        <v>302.01</v>
+      </c>
+    </row>
+    <row r="63" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="AZ63">
+        <f>AZ60+AZ61+AZ62</f>
+        <v>19377.313400000003</v>
+      </c>
+    </row>
+    <row r="64" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="AZ64">
+        <f>SUM(AZ2:AZ56)</f>
+        <v>19377.313400000003</v>
+      </c>
+    </row>
+    <row r="65" spans="52:52" x14ac:dyDescent="0.2">
+      <c r="AZ65">
+        <f>AZ61+AZ60</f>
+        <v>9285.9134000000013</v>
       </c>
     </row>
   </sheetData>
@@ -41297,10 +44013,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB57"/>
+  <dimension ref="A1:BB65"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C56"/>
+      <selection activeCell="J62" sqref="J62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -49817,6 +52533,567 @@
       </c>
       <c r="AY57">
         <v>-999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="I60" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="J60">
+        <f>SUM(J2:J3,J5:J14,J17:J20,J24:J32,J34,J36,J39,J41:J54,J56)</f>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="K60">
+        <f t="shared" ref="K60:AX60" si="4">SUM(K2:K3,K5:K14,K17:K20,K24:K32,K34,K36,K39,K41:K54,K56)</f>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="M60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="O60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="P60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="Q60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="R60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="S60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="T60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="U60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="V60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="W60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="X60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="Y60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="Z60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="AA60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="AB60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="AC60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="AD60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="AE60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="AF60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="AG60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="AH60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="AI60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="AJ60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="AK60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="AL60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="AM60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="AN60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="AO60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="AP60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="AQ60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="AR60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="AS60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="AT60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="AU60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="AV60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="AW60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="AX60">
+        <f t="shared" si="4"/>
+        <v>533.95228999999995</v>
+      </c>
+      <c r="AZ60">
+        <f t="shared" ref="AZ60:BB60" si="5">SUM(AZ2:AZ3,AZ5:AZ14,AZ17:AZ20,AZ24:AZ32,AZ34,AZ36,AZ39,AZ41:AZ54,AZ56)</f>
+        <v>533.95229000000006</v>
+      </c>
+      <c r="BA60">
+        <f t="shared" si="5"/>
+        <v>8627.671362317109</v>
+      </c>
+      <c r="BB60">
+        <f t="shared" si="5"/>
+        <v>198.85098909090908</v>
+      </c>
+    </row>
+    <row r="61" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="I61" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="J61">
+        <f>SUM(J4,J15:J16,J33,J35,J37:J38,J40,J55)</f>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="K61">
+        <f t="shared" ref="K61:AX61" si="6">SUM(K4,K15:K16,K33,K35,K37:K38,K40,K55)</f>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="M61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="P61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="Q61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="R61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="S61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="T61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="U61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="V61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="W61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="X61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="Y61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="Z61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="AA61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="AB61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="AC61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="AD61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="AE61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="AF61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="AG61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="AH61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="AI61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="AJ61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="AK61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="AL61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="AM61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="AN61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="AO61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="AP61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="AQ61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="AR61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="AS61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="AT61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="AU61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="AV61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="AW61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="AX61">
+        <f t="shared" si="6"/>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="AZ61">
+        <f t="shared" ref="AZ61:BB61" si="7">SUM(AZ4,AZ15:AZ16,AZ33,AZ35,AZ37:AZ38,AZ40,AZ55)</f>
+        <v>267.66000000000003</v>
+      </c>
+      <c r="BA61">
+        <f t="shared" si="7"/>
+        <v>2784.6499776736705</v>
+      </c>
+      <c r="BB61">
+        <f t="shared" si="7"/>
+        <v>76.96141636363636</v>
+      </c>
+    </row>
+    <row r="62" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="I62" t="s">
+        <v>73</v>
+      </c>
+      <c r="J62">
+        <f>SUM(J21:J23)</f>
+        <v>1080.75</v>
+      </c>
+      <c r="K62">
+        <f t="shared" ref="K62:AX62" si="8">SUM(K21:K23)</f>
+        <v>1080.75</v>
+      </c>
+      <c r="L62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="M62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="N62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="O62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="P62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="Q62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="R62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="S62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="T62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="U62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="V62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="W62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="X62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="Y62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="Z62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="AA62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="AB62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="AC62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="AD62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="AE62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="AF62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="AG62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="AH62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="AI62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="AJ62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="AK62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="AL62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="AM62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="AN62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="AO62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="AP62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="AQ62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="AR62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="AS62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="AT62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="AU62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="AV62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="AW62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="AX62">
+        <f t="shared" si="8"/>
+        <v>1080.75</v>
+      </c>
+      <c r="AZ62">
+        <f t="shared" ref="AZ62:BB62" si="9">SUM(AZ21:AZ23)</f>
+        <v>1080.75</v>
+      </c>
+      <c r="BA62">
+        <f t="shared" si="9"/>
+        <v>766.8265478437329</v>
+      </c>
+      <c r="BB62">
+        <f t="shared" si="9"/>
+        <v>302.01</v>
+      </c>
+    </row>
+    <row r="63" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="AZ63">
+        <f>AZ60+AZ61+AZ62</f>
+        <v>1882.36229</v>
+      </c>
+    </row>
+    <row r="64" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="AZ64">
+        <f>SUM(AZ2:AZ56)</f>
+        <v>1882.3622900000005</v>
+      </c>
+    </row>
+    <row r="65" spans="52:52" x14ac:dyDescent="0.2">
+      <c r="AZ65">
+        <f>AZ61+AZ60</f>
+        <v>801.61229000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>